<commit_message>
Alterado o cy.wait em algumas telas
</commit_message>
<xml_diff>
--- a/cypress/downloads/Taxas.xlsx
+++ b/cypress/downloads/Taxas.xlsx
@@ -486,28 +486,26 @@
     </row>
     <row r="13" spans="1:8" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>13</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="D13" s="3" t="s"/>
       <c r="E13" s="4" t="n">
         <v>1</v>
       </c>
       <c r="F13" s="4" t="n">
-        <v>2</v>
+        <v>2.4</v>
       </c>
       <c r="G13" s="5" t="n">
-        <v>45111</v>
+        <v>44927</v>
       </c>
       <c r="H13" s="5" t="n">
-        <v>45113</v>
+        <v>45291</v>
       </c>
     </row>
     <row r="14" spans="1:8" outlineLevel="0" x14ac:dyDescent="0.25">
@@ -562,26 +560,28 @@
     </row>
     <row r="16" spans="1:8" outlineLevel="0" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D16" s="3" t="s"/>
+        <v>12</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="E16" s="4" t="n">
         <v>1</v>
       </c>
       <c r="F16" s="4" t="n">
-        <v>2.4</v>
+        <v>2</v>
       </c>
       <c r="G16" s="5" t="n">
-        <v>44927</v>
+        <v>45111</v>
       </c>
       <c r="H16" s="5" t="n">
-        <v>45291</v>
+        <v>45113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>